<commit_message>
Add GER field to courses.json
</commit_message>
<xml_diff>
--- a/src/spz/spz/templates/export/spanisch.xlsx
+++ b/src/spz/spz/templates/export/spanisch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\spz-signup\src\spz\spz\templates\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64A021C-9B37-4ABA-A34F-A653E61E7378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22870436-14FC-46B5-AF3F-F9A723060053}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,8 @@
     <sheet name="Paricipantlist" sheetId="12" r:id="rId5"/>
     <sheet name="Teilnehmer" sheetId="13" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="Anmeldestatus">[1]Tabelle2!$A$1:$A$2</definedName>
     <definedName name="kursname">Notenliste!$A$42:$A$50</definedName>
-    <definedName name="Notenskala">[1]Tabelle2!$B$1:$B$13</definedName>
     <definedName name="semester">Notenliste!$D$42:$D$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -244,9 +239,6 @@
   </si>
   <si>
     <t>C1</t>
-  </si>
-  <si>
-    <t>Elena Moya Royo</t>
   </si>
   <si>
     <t>Prüfungsdatum</t>
@@ -1157,93 +1149,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Teilnehmer"/>
-      <sheetName val="Tabelle2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>angemeldet</v>
-          </cell>
-          <cell r="B1">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>abgemeldet</v>
-          </cell>
-          <cell r="B2">
-            <v>1.3</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>1.7</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>2.7</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>3.3</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>3.7</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v>bestanden</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>nicht bestanden</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1665,22 +1570,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>62</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1946,8 +1851,8 @@
   </sheetPr>
   <dimension ref="A1:WVW61"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView showZeros="0" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.3" zeroHeight="1" x14ac:dyDescent="0.4"/>
@@ -3908,9 +3813,7 @@
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="B31" s="10"/>
       <c r="C31" s="26"/>
       <c r="D31" s="77" t="s">
         <v>34</v>
@@ -3965,7 +3868,7 @@
         <v>17</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="77"/>
@@ -3983,7 +3886,7 @@
         <v>43</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="77"/>
@@ -3998,10 +3901,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="77"/>
@@ -4034,7 +3937,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="68">
         <v>43496</v>
@@ -4282,7 +4185,7 @@
   </sheetPr>
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -4323,7 +4226,7 @@
     <row r="2" spans="1:14" s="66" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="80" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B31</f>
-        <v>Dozent/in: Elena Moya Royo</v>
+        <v xml:space="preserve">Dozent/in: </v>
       </c>
       <c r="B2" s="80"/>
       <c r="C2" s="80"/>
@@ -6022,7 +5925,7 @@
     <row r="3" spans="1:24" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="87" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B31</f>
-        <v>Dozent/in: Elena Moya Royo</v>
+        <v xml:space="preserve">Dozent/in: </v>
       </c>
       <c r="B3" s="87"/>
       <c r="C3" s="87"/>
@@ -7194,25 +7097,25 @@
         <v>27</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
       </c>
       <c r="D1" s="70" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>52</v>
-      </c>
-      <c r="H1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">

</xml_diff>